<commit_message>
Abs.: Aufbau der Evaluation
</commit_message>
<xml_diff>
--- a/Auswertungen/Usability Evaluation- Masterthesis.xlsx
+++ b/Auswertungen/Usability Evaluation- Masterthesis.xlsx
@@ -1210,6 +1210,8 @@
     <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1218,8 +1220,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1688,13 +1688,13 @@
       <c r="K2" s="2">
         <v>4</v>
       </c>
-      <c r="L2" s="41">
+      <c r="L2" s="37">
         <v>4</v>
       </c>
-      <c r="M2" s="41">
+      <c r="M2" s="37">
         <v>2</v>
       </c>
-      <c r="N2" s="41">
+      <c r="N2" s="37">
         <v>3</v>
       </c>
       <c r="O2" s="2">
@@ -1780,13 +1780,13 @@
       <c r="K3" s="2">
         <v>4</v>
       </c>
-      <c r="L3" s="41">
+      <c r="L3" s="37">
         <v>5</v>
       </c>
-      <c r="M3" s="41">
+      <c r="M3" s="37">
         <v>4</v>
       </c>
-      <c r="N3" s="41">
+      <c r="N3" s="37">
         <v>3</v>
       </c>
       <c r="O3" s="2">
@@ -1869,13 +1869,13 @@
       <c r="J4" s="2">
         <v>0</v>
       </c>
-      <c r="L4" s="41">
+      <c r="L4" s="37">
         <v>5</v>
       </c>
-      <c r="M4" s="41">
+      <c r="M4" s="37">
         <v>2</v>
       </c>
-      <c r="N4" s="41">
+      <c r="N4" s="37">
         <v>4</v>
       </c>
       <c r="O4" s="2">
@@ -1958,13 +1958,13 @@
       <c r="K5" s="2">
         <v>5</v>
       </c>
-      <c r="L5" s="41">
+      <c r="L5" s="37">
         <v>4</v>
       </c>
-      <c r="M5" s="41">
+      <c r="M5" s="37">
         <v>2</v>
       </c>
-      <c r="N5" s="41">
+      <c r="N5" s="37">
         <v>2</v>
       </c>
       <c r="O5" s="2">
@@ -2050,13 +2050,13 @@
       <c r="J6" s="34">
         <v>0</v>
       </c>
-      <c r="L6" s="41">
+      <c r="L6" s="37">
         <v>5</v>
       </c>
-      <c r="M6" s="41">
+      <c r="M6" s="37">
         <v>2</v>
       </c>
-      <c r="N6" s="41">
+      <c r="N6" s="37">
         <v>1</v>
       </c>
       <c r="O6" s="2">
@@ -2145,13 +2145,13 @@
       <c r="J7" s="2">
         <v>0</v>
       </c>
-      <c r="L7" s="41">
+      <c r="L7" s="37">
         <v>5</v>
       </c>
-      <c r="M7" s="41">
+      <c r="M7" s="37">
         <v>1</v>
       </c>
-      <c r="N7" s="41">
+      <c r="N7" s="37">
         <v>1</v>
       </c>
       <c r="O7" s="2">
@@ -2240,13 +2240,13 @@
       <c r="J8" s="2">
         <v>0</v>
       </c>
-      <c r="L8" s="41">
+      <c r="L8" s="37">
         <v>4</v>
       </c>
-      <c r="M8" s="41">
+      <c r="M8" s="37">
         <v>4</v>
       </c>
-      <c r="N8" s="41">
+      <c r="N8" s="37">
         <v>1</v>
       </c>
       <c r="O8" s="2">
@@ -2332,13 +2332,13 @@
       <c r="J9" s="2">
         <v>0</v>
       </c>
-      <c r="L9" s="41">
+      <c r="L9" s="37">
         <v>4</v>
       </c>
-      <c r="M9" s="41">
+      <c r="M9" s="37">
         <v>2</v>
       </c>
-      <c r="N9" s="41">
+      <c r="N9" s="37">
         <v>4</v>
       </c>
       <c r="O9" s="2">
@@ -2421,13 +2421,13 @@
       <c r="J10" s="2">
         <v>0</v>
       </c>
-      <c r="L10" s="41">
+      <c r="L10" s="37">
         <v>5</v>
       </c>
-      <c r="M10" s="41">
+      <c r="M10" s="37">
         <v>4</v>
       </c>
-      <c r="N10" s="41">
+      <c r="N10" s="37">
         <v>1</v>
       </c>
       <c r="O10" s="2">
@@ -2519,13 +2519,13 @@
       <c r="K11" s="2">
         <v>4</v>
       </c>
-      <c r="L11" s="41">
+      <c r="L11" s="37">
         <v>5</v>
       </c>
-      <c r="M11" s="41">
+      <c r="M11" s="37">
         <v>2</v>
       </c>
-      <c r="N11" s="41">
+      <c r="N11" s="37">
         <v>1</v>
       </c>
       <c r="O11" s="2">
@@ -2612,13 +2612,13 @@
       <c r="K12" s="17">
         <v>4</v>
       </c>
-      <c r="L12" s="42">
+      <c r="L12" s="38">
         <v>5</v>
       </c>
-      <c r="M12" s="42">
+      <c r="M12" s="38">
         <v>3</v>
       </c>
-      <c r="N12" s="42">
+      <c r="N12" s="38">
         <v>2</v>
       </c>
       <c r="O12" s="17">
@@ -9252,52 +9252,52 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="37" t="s">
+      <c r="B1" s="39" t="s">
         <v>23</v>
       </c>
       <c r="C1" s="19"/>
-      <c r="D1" s="37" t="s">
+      <c r="D1" s="39" t="s">
         <v>109</v>
       </c>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="H1" s="37" t="s">
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
+      <c r="H1" s="39" t="s">
         <v>110</v>
       </c>
-      <c r="I1" s="38"/>
-      <c r="J1" s="38"/>
-      <c r="K1" s="39" t="s">
+      <c r="I1" s="40"/>
+      <c r="J1" s="40"/>
+      <c r="K1" s="41" t="s">
         <v>111</v>
       </c>
-      <c r="L1" s="38"/>
-      <c r="M1" s="38"/>
-      <c r="O1" s="37" t="s">
+      <c r="L1" s="40"/>
+      <c r="M1" s="40"/>
+      <c r="O1" s="39" t="s">
         <v>112</v>
       </c>
-      <c r="P1" s="38"/>
-      <c r="Q1" s="38"/>
-      <c r="R1" s="39" t="s">
+      <c r="P1" s="40"/>
+      <c r="Q1" s="40"/>
+      <c r="R1" s="41" t="s">
         <v>113</v>
       </c>
-      <c r="S1" s="38"/>
-      <c r="T1" s="38"/>
-      <c r="U1" s="39" t="s">
+      <c r="S1" s="40"/>
+      <c r="T1" s="40"/>
+      <c r="U1" s="41" t="s">
         <v>114</v>
       </c>
-      <c r="V1" s="38"/>
-      <c r="W1" s="38"/>
-      <c r="X1" s="39" t="s">
+      <c r="V1" s="40"/>
+      <c r="W1" s="40"/>
+      <c r="X1" s="41" t="s">
         <v>115</v>
       </c>
-      <c r="Y1" s="38"/>
-      <c r="Z1" s="38"/>
+      <c r="Y1" s="40"/>
+      <c r="Z1" s="40"/>
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A2" s="38"/>
-      <c r="B2" s="38"/>
+      <c r="A2" s="40"/>
+      <c r="B2" s="40"/>
       <c r="C2" s="32" t="s">
         <v>125</v>
       </c>

</xml_diff>

<commit_message>
update: Auswertung Verhalten der Darstellungsformen
</commit_message>
<xml_diff>
--- a/Auswertungen/Usability Evaluation- Masterthesis.xlsx
+++ b/Auswertungen/Usability Evaluation- Masterthesis.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11760" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12000" windowHeight="5280" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Formularantworten 1" sheetId="1" r:id="rId1"/>
@@ -868,7 +868,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1050" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1096" uniqueCount="217">
   <si>
     <t>Testperson</t>
   </si>
@@ -1516,6 +1516,12 @@
     <t>Verwendung der verschiedenen Ansichten 
 (Mittelwert Gruppe)</t>
   </si>
+  <si>
+    <t>Häufigkeit der Verwendung (Summe Gesamt)</t>
+  </si>
+  <si>
+    <t>Häufigkeit der Verwendung (Mittelwert Gruppe)</t>
+  </si>
 </sst>
 </file>
 
@@ -1608,7 +1614,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -1686,6 +1692,9 @@
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="166" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="167" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1700,11 +1709,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1756,11 +1763,19 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="de-AT"/>
+              <a:rPr lang="de-AT">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:rPr>
               <a:t>Bearbeitungsdauer der Trips</a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="de-AT" baseline="0"/>
+              <a:rPr lang="de-AT" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:rPr>
               <a:t> (Mittelwert Gruppe)</a:t>
             </a:r>
           </a:p>
@@ -1900,6 +1915,7 @@
               <a:solidFill>
                 <a:schemeClr val="accent5"/>
               </a:solidFill>
+              <a:prstDash val="dash"/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -1982,6 +1998,7 @@
                   <a:lumMod val="60000"/>
                 </a:schemeClr>
               </a:solidFill>
+              <a:prstDash val="sysDot"/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -2705,12 +2722,9 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -2768,8 +2782,12 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="de-AT"/>
-                  <a:t>Bearbeitungsdauer in Min.</a:t>
+                  <a:rPr lang="de-AT" sz="1200">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>Bearbeitungsdauer  [Min:Sec]</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -2863,10 +2881,7 @@
           <a:pPr>
             <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
@@ -2948,8 +2963,28 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="de-AT"/>
-              <a:t>Verwendung der verschiedenen Ansichten </a:t>
+              <a:rPr lang="de-AT">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Verwendungsdauer</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="de-AT" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t> der </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="de-AT">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Ansichten</a:t>
             </a:r>
           </a:p>
           <a:p>
@@ -2957,7 +2992,11 @@
               <a:defRPr/>
             </a:pPr>
             <a:r>
-              <a:rPr lang="de-AT"/>
+              <a:rPr lang="de-AT">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:rPr>
               <a:t>(Mittelwert Gruppe)</a:t>
             </a:r>
           </a:p>
@@ -3305,12 +3344,9 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -3348,6 +3384,108 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+                  <a:lnSpc>
+                    <a:spcPct val="100000"/>
+                  </a:lnSpc>
+                  <a:spcBef>
+                    <a:spcPts val="0"/>
+                  </a:spcBef>
+                  <a:spcAft>
+                    <a:spcPts val="0"/>
+                  </a:spcAft>
+                  <a:buClrTx/>
+                  <a:buSzTx/>
+                  <a:buFontTx/>
+                  <a:buNone/>
+                  <a:tabLst/>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:sysClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-AT" sz="1200" b="0" i="0" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>Verwendungsdauer [Std:Min:Sec]</a:t>
+                </a:r>
+                <a:endParaRPr lang="de-AT" sz="700">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:effectLst/>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="9.9259608089370295E-3"/>
+              <c:y val="0.15145465239424483"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr marL="0" marR="0" lvl="0" indent="0" algn="ctr" defTabSz="914400" rtl="0" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+                <a:lnSpc>
+                  <a:spcPct val="100000"/>
+                </a:lnSpc>
+                <a:spcBef>
+                  <a:spcPts val="0"/>
+                </a:spcBef>
+                <a:spcAft>
+                  <a:spcPts val="0"/>
+                </a:spcAft>
+                <a:buClrTx/>
+                <a:buSzTx/>
+                <a:buFontTx/>
+                <a:buNone/>
+                <a:tabLst/>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:sysClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="de-DE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="h:mm:ss;@" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -3406,12 +3544,9 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
@@ -3493,11 +3628,19 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="de-AT"/>
-              <a:t>Verwendung der</a:t>
+              <a:rPr lang="de-AT">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Verwendungsdauer der</a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="de-AT" baseline="0"/>
+              <a:rPr lang="de-AT" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:rPr>
               <a:t> Ansichten</a:t>
             </a:r>
           </a:p>
@@ -3506,10 +3649,18 @@
               <a:defRPr/>
             </a:pPr>
             <a:r>
-              <a:rPr lang="de-AT" baseline="0"/>
+              <a:rPr lang="de-AT" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:rPr>
               <a:t>(Gesamt nach Trip)</a:t>
             </a:r>
-            <a:endParaRPr lang="de-AT"/>
+            <a:endParaRPr lang="de-AT">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:endParaRPr>
           </a:p>
         </c:rich>
       </c:tx>
@@ -3567,6 +3718,7 @@
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
+              <a:prstDash val="dash"/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -3647,6 +3799,7 @@
               <a:solidFill>
                 <a:schemeClr val="accent2"/>
               </a:solidFill>
+              <a:prstDash val="sysDot"/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -3750,12 +3903,9 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -3793,6 +3943,86 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-AT" sz="1200">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>Verwendungsdauer</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="de-AT" sz="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t> [Std:Min:Sec]</a:t>
+                </a:r>
+                <a:endParaRPr lang="de-AT" sz="1200">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="1.8781564489533345E-2"/>
+              <c:y val="0.11995325386397541"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="de-DE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="h:mm:ss;@" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -3851,12 +4081,9 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
@@ -3905,6 +4132,599 @@
 </file>
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="de-DE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="de-AT">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Häufigkeit der Verwendung (Mittelwert Gruppe)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Darstellungsformen!$H$39</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Karte</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>Darstellungsformen!$F$40:$G$48</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="9"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Gruppe 1</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Gruppe 2</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>Gruppe 3</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Gruppe 1</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>Gruppe 2</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>Gruppe 3</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>Gruppe 1</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>Gruppe 2</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>Gruppe 3</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Trip 1</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Trip 1</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>Trip 1</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Trip 2</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>Trip 2</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>Trip 2</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>Trip 3</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>Trip 3</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>Trip 3</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Darstellungsformen!$H$40:$H$48</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1.3333333333333333</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.3333333333333333</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.3333333333333333</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.6666666666666667</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-8C49-489B-A0FD-A521FC107E82}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Darstellungsformen!$I$39</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Liste</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>Darstellungsformen!$F$40:$G$48</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="9"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Gruppe 1</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Gruppe 2</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>Gruppe 3</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Gruppe 1</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>Gruppe 2</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>Gruppe 3</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>Gruppe 1</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>Gruppe 2</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>Gruppe 3</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Trip 1</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Trip 1</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>Trip 1</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Trip 2</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>Trip 2</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>Trip 2</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>Trip 3</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>Trip 3</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>Trip 3</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Darstellungsformen!$I$40:$I$48</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.3333333333333333</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.6666666666666667</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.3333333333333333</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-8C49-489B-A0FD-A521FC107E82}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1191817040"/>
+        <c:axId val="1191804560"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1191817040"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1191804560"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1191804560"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-AT" sz="1200">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>Anzahl</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="de-DE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1191817040"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="de-DE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="de-DE"/>
@@ -4755,7 +5575,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="de-DE"/>
@@ -5530,7 +6350,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="de-DE"/>
@@ -6603,10 +7423,13 @@
 </file>
 
 <file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="13">
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
   <a:schemeClr val="accent6"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent4"/>
   <cs:variation/>
   <cs:variation>
     <a:lumMod val="60000"/>
@@ -6677,6 +7500,43 @@
 </file>
 
 <file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="13">
+  <a:schemeClr val="accent6"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent4"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="13">
   <a:schemeClr val="accent6"/>
   <a:schemeClr val="accent5"/>
@@ -8236,7 +9096,7 @@
 </file>
 
 <file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -8344,11 +9204,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
@@ -8359,11 +9214,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
@@ -8395,9 +9245,6 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -9783,20 +10630,536 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>162983</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>162983</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:rowOff>84667</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -9819,12 +11182,12 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>495300</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>80682</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>238125</xdr:colOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>446515</xdr:colOff>
       <xdr:row>36</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
@@ -9847,16 +11210,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>57150</xdr:colOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>400797</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>76698</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>400797</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>58769</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -9870,6 +11233,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>502022</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>681317</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Diagramm 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -10284,18 +11677,18 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="7" width="21.5703125" customWidth="1"/>
-    <col min="8" max="11" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="14" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="19" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="7" width="21.5546875" customWidth="1"/>
+    <col min="8" max="11" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="14" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="19" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="20" max="24" width="11" bestFit="1" customWidth="1"/>
-    <col min="25" max="27" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="28.5703125" customWidth="1"/>
-    <col min="29" max="29" width="21.5703125" customWidth="1"/>
+    <col min="25" max="27" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="28.5546875" customWidth="1"/>
+    <col min="29" max="29" width="21.5546875" customWidth="1"/>
     <col min="30" max="30" width="108" customWidth="1"/>
-    <col min="31" max="31" width="95.5703125" customWidth="1"/>
+    <col min="31" max="31" width="95.5546875" customWidth="1"/>
     <col min="32" max="32" width="15" customWidth="1"/>
   </cols>
   <sheetData>
@@ -11705,9 +13098,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2"/>
   <cols>
-    <col min="9" max="9" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.33203125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="21" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -12373,12 +13766,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2"/>
   <cols>
-    <col min="4" max="6" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="21" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.7109375" customWidth="1"/>
+    <col min="9" max="9" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -12950,9 +14343,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="3" max="3" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="15.75" customHeight="1">
@@ -13108,20 +14501,19 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:P179"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView topLeftCell="A2" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="3" max="3" width="9" customWidth="1"/>
-    <col min="18" max="18" width="29.42578125" customWidth="1"/>
+    <col min="18" max="18" width="29.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="12.75">
+    <row r="1" spans="1:16" ht="13.2">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -13166,7 +14558,7 @@
       </c>
       <c r="O1" s="33"/>
     </row>
-    <row r="2" spans="1:16" ht="14.25" hidden="1">
+    <row r="2" spans="1:16" ht="13.8">
       <c r="A2" s="6" t="s">
         <v>37</v>
       </c>
@@ -13205,7 +14597,7 @@
       </c>
       <c r="P2" s="28"/>
     </row>
-    <row r="3" spans="1:16" ht="14.25" hidden="1">
+    <row r="3" spans="1:16" ht="13.8">
       <c r="A3" s="6" t="s">
         <v>37</v>
       </c>
@@ -13247,7 +14639,7 @@
       </c>
       <c r="P3" s="28"/>
     </row>
-    <row r="4" spans="1:16" ht="14.25" hidden="1">
+    <row r="4" spans="1:16" ht="13.8">
       <c r="A4" s="6" t="s">
         <v>37</v>
       </c>
@@ -13289,7 +14681,7 @@
       </c>
       <c r="P4" s="28"/>
     </row>
-    <row r="5" spans="1:16" ht="14.25" hidden="1">
+    <row r="5" spans="1:16" ht="13.8">
       <c r="A5" s="6" t="s">
         <v>37</v>
       </c>
@@ -13331,7 +14723,7 @@
       </c>
       <c r="P5" s="28"/>
     </row>
-    <row r="6" spans="1:16" ht="14.25" hidden="1">
+    <row r="6" spans="1:16" ht="13.8">
       <c r="A6" s="6" t="s">
         <v>37</v>
       </c>
@@ -13373,7 +14765,7 @@
       </c>
       <c r="P6" s="28"/>
     </row>
-    <row r="7" spans="1:16" ht="14.25" hidden="1">
+    <row r="7" spans="1:16" ht="13.8">
       <c r="A7" s="6" t="s">
         <v>37</v>
       </c>
@@ -13413,7 +14805,7 @@
       </c>
       <c r="P7" s="28"/>
     </row>
-    <row r="8" spans="1:16" ht="14.25" hidden="1">
+    <row r="8" spans="1:16" ht="13.8">
       <c r="A8" s="2" t="s">
         <v>37</v>
       </c>
@@ -13448,7 +14840,7 @@
       </c>
       <c r="P8" s="28"/>
     </row>
-    <row r="9" spans="1:16" ht="14.25" hidden="1">
+    <row r="9" spans="1:16" ht="13.8">
       <c r="A9" s="2" t="s">
         <v>37</v>
       </c>
@@ -13486,7 +14878,7 @@
       </c>
       <c r="P9" s="28"/>
     </row>
-    <row r="10" spans="1:16" ht="14.25" hidden="1">
+    <row r="10" spans="1:16" ht="13.8">
       <c r="A10" s="2" t="s">
         <v>37</v>
       </c>
@@ -13524,7 +14916,7 @@
       </c>
       <c r="P10" s="28"/>
     </row>
-    <row r="11" spans="1:16" ht="14.25" hidden="1">
+    <row r="11" spans="1:16" ht="13.8">
       <c r="A11" s="2" t="s">
         <v>37</v>
       </c>
@@ -13562,7 +14954,7 @@
       </c>
       <c r="P11" s="28"/>
     </row>
-    <row r="12" spans="1:16" ht="14.25" hidden="1">
+    <row r="12" spans="1:16" ht="13.8">
       <c r="A12" s="2" t="s">
         <v>37</v>
       </c>
@@ -13597,7 +14989,7 @@
       </c>
       <c r="P12" s="28"/>
     </row>
-    <row r="13" spans="1:16" ht="14.25" hidden="1">
+    <row r="13" spans="1:16" ht="13.8">
       <c r="A13" s="6" t="s">
         <v>37</v>
       </c>
@@ -13637,7 +15029,7 @@
       </c>
       <c r="P13" s="28"/>
     </row>
-    <row r="14" spans="1:16" ht="14.25" hidden="1">
+    <row r="14" spans="1:16" ht="13.8">
       <c r="A14" s="6" t="s">
         <v>37</v>
       </c>
@@ -13679,7 +15071,7 @@
       </c>
       <c r="P14" s="28"/>
     </row>
-    <row r="15" spans="1:16" ht="14.25" hidden="1">
+    <row r="15" spans="1:16" ht="13.8">
       <c r="A15" s="6" t="s">
         <v>37</v>
       </c>
@@ -13721,7 +15113,7 @@
       </c>
       <c r="P15" s="28"/>
     </row>
-    <row r="16" spans="1:16" ht="14.25" hidden="1">
+    <row r="16" spans="1:16" ht="13.8">
       <c r="A16" s="6" t="s">
         <v>37</v>
       </c>
@@ -13763,7 +15155,7 @@
       </c>
       <c r="P16" s="28"/>
     </row>
-    <row r="17" spans="1:16" ht="14.25" hidden="1">
+    <row r="17" spans="1:16" ht="13.8">
       <c r="A17" s="6" t="s">
         <v>37</v>
       </c>
@@ -13803,7 +15195,7 @@
       </c>
       <c r="P17" s="28"/>
     </row>
-    <row r="18" spans="1:16" ht="14.25" hidden="1">
+    <row r="18" spans="1:16" ht="13.8">
       <c r="A18" s="2" t="s">
         <v>54</v>
       </c>
@@ -13838,7 +15230,7 @@
       </c>
       <c r="P18" s="28"/>
     </row>
-    <row r="19" spans="1:16" ht="14.25" hidden="1">
+    <row r="19" spans="1:16" ht="13.8">
       <c r="A19" s="2" t="s">
         <v>54</v>
       </c>
@@ -13876,7 +15268,7 @@
       </c>
       <c r="P19" s="28"/>
     </row>
-    <row r="20" spans="1:16" ht="14.25" hidden="1">
+    <row r="20" spans="1:16" ht="13.8">
       <c r="A20" s="2" t="s">
         <v>54</v>
       </c>
@@ -13914,7 +15306,7 @@
       </c>
       <c r="P20" s="28"/>
     </row>
-    <row r="21" spans="1:16" ht="14.25" hidden="1">
+    <row r="21" spans="1:16" ht="13.8">
       <c r="A21" s="2" t="s">
         <v>54</v>
       </c>
@@ -13952,7 +15344,7 @@
       </c>
       <c r="P21" s="28"/>
     </row>
-    <row r="22" spans="1:16" ht="14.25" hidden="1">
+    <row r="22" spans="1:16" ht="13.8">
       <c r="A22" s="2" t="s">
         <v>54</v>
       </c>
@@ -13990,7 +15382,7 @@
       </c>
       <c r="P22" s="28"/>
     </row>
-    <row r="23" spans="1:16" ht="14.25" hidden="1">
+    <row r="23" spans="1:16" ht="13.8">
       <c r="A23" s="2" t="s">
         <v>54</v>
       </c>
@@ -14025,7 +15417,7 @@
       </c>
       <c r="P23" s="28"/>
     </row>
-    <row r="24" spans="1:16" ht="14.25" hidden="1">
+    <row r="24" spans="1:16" ht="13.8">
       <c r="A24" s="6" t="s">
         <v>54</v>
       </c>
@@ -14065,7 +15457,7 @@
       </c>
       <c r="P24" s="28"/>
     </row>
-    <row r="25" spans="1:16" ht="14.25" hidden="1">
+    <row r="25" spans="1:16" ht="13.8">
       <c r="A25" s="6" t="s">
         <v>54</v>
       </c>
@@ -14107,7 +15499,7 @@
       </c>
       <c r="P25" s="28"/>
     </row>
-    <row r="26" spans="1:16" ht="14.25" hidden="1">
+    <row r="26" spans="1:16" ht="13.8">
       <c r="A26" s="6" t="s">
         <v>54</v>
       </c>
@@ -14149,7 +15541,7 @@
       </c>
       <c r="P26" s="28"/>
     </row>
-    <row r="27" spans="1:16" ht="14.25" hidden="1">
+    <row r="27" spans="1:16" ht="13.8">
       <c r="A27" s="6" t="s">
         <v>54</v>
       </c>
@@ -14191,7 +15583,7 @@
       </c>
       <c r="P27" s="28"/>
     </row>
-    <row r="28" spans="1:16" ht="14.25" hidden="1">
+    <row r="28" spans="1:16" ht="13.8">
       <c r="A28" s="6" t="s">
         <v>54</v>
       </c>
@@ -14233,7 +15625,7 @@
       </c>
       <c r="P28" s="28"/>
     </row>
-    <row r="29" spans="1:16" ht="14.25" hidden="1">
+    <row r="29" spans="1:16" ht="13.8">
       <c r="A29" s="6" t="s">
         <v>54</v>
       </c>
@@ -14273,7 +15665,7 @@
       </c>
       <c r="P29" s="28"/>
     </row>
-    <row r="30" spans="1:16" ht="14.25" hidden="1">
+    <row r="30" spans="1:16" ht="13.8">
       <c r="A30" s="2" t="s">
         <v>54</v>
       </c>
@@ -14308,7 +15700,7 @@
       </c>
       <c r="P30" s="28"/>
     </row>
-    <row r="31" spans="1:16" ht="14.25" hidden="1">
+    <row r="31" spans="1:16" ht="13.8">
       <c r="A31" s="2" t="s">
         <v>54</v>
       </c>
@@ -14346,7 +15738,7 @@
       </c>
       <c r="P31" s="28"/>
     </row>
-    <row r="32" spans="1:16" ht="14.25" hidden="1">
+    <row r="32" spans="1:16" ht="13.8">
       <c r="A32" s="2" t="s">
         <v>54</v>
       </c>
@@ -14384,7 +15776,7 @@
       </c>
       <c r="P32" s="28"/>
     </row>
-    <row r="33" spans="1:16" ht="14.25" hidden="1">
+    <row r="33" spans="1:16" ht="13.8">
       <c r="A33" s="2" t="s">
         <v>54</v>
       </c>
@@ -14422,7 +15814,7 @@
       </c>
       <c r="P33" s="28"/>
     </row>
-    <row r="34" spans="1:16" ht="14.25" hidden="1">
+    <row r="34" spans="1:16" ht="13.8">
       <c r="A34" s="2" t="s">
         <v>54</v>
       </c>
@@ -14460,7 +15852,7 @@
       </c>
       <c r="P34" s="28"/>
     </row>
-    <row r="35" spans="1:16" ht="14.25" hidden="1">
+    <row r="35" spans="1:16" ht="13.8">
       <c r="A35" s="2" t="s">
         <v>54</v>
       </c>
@@ -14495,7 +15887,7 @@
       </c>
       <c r="P35" s="28"/>
     </row>
-    <row r="36" spans="1:16" ht="14.25">
+    <row r="36" spans="1:16" ht="13.8">
       <c r="A36" s="6" t="s">
         <v>62</v>
       </c>
@@ -14535,7 +15927,7 @@
       </c>
       <c r="P36" s="28"/>
     </row>
-    <row r="37" spans="1:16" ht="14.25">
+    <row r="37" spans="1:16" ht="13.8">
       <c r="A37" s="6" t="s">
         <v>62</v>
       </c>
@@ -14577,7 +15969,7 @@
       </c>
       <c r="P37" s="28"/>
     </row>
-    <row r="38" spans="1:16" ht="14.25">
+    <row r="38" spans="1:16" ht="13.8">
       <c r="A38" s="6" t="s">
         <v>62</v>
       </c>
@@ -14619,7 +16011,7 @@
       </c>
       <c r="P38" s="28"/>
     </row>
-    <row r="39" spans="1:16" ht="14.25">
+    <row r="39" spans="1:16" ht="13.8">
       <c r="A39" s="6" t="s">
         <v>62</v>
       </c>
@@ -14660,7 +16052,7 @@
         <v>group1</v>
       </c>
     </row>
-    <row r="40" spans="1:16" ht="14.25">
+    <row r="40" spans="1:16" ht="13.8">
       <c r="A40" s="6" t="s">
         <v>62</v>
       </c>
@@ -14699,7 +16091,7 @@
         <v>group1</v>
       </c>
     </row>
-    <row r="41" spans="1:16" ht="14.25" hidden="1">
+    <row r="41" spans="1:16" ht="13.8">
       <c r="A41" s="2" t="s">
         <v>62</v>
       </c>
@@ -14733,7 +16125,7 @@
         <v>group1</v>
       </c>
     </row>
-    <row r="42" spans="1:16" ht="14.25" hidden="1">
+    <row r="42" spans="1:16" ht="13.8">
       <c r="A42" s="2" t="s">
         <v>62</v>
       </c>
@@ -14770,7 +16162,7 @@
         <v>group1</v>
       </c>
     </row>
-    <row r="43" spans="1:16" ht="14.25" hidden="1">
+    <row r="43" spans="1:16" ht="13.8">
       <c r="A43" s="2" t="s">
         <v>62</v>
       </c>
@@ -14807,7 +16199,7 @@
         <v>group1</v>
       </c>
     </row>
-    <row r="44" spans="1:16" ht="14.25" hidden="1">
+    <row r="44" spans="1:16" ht="13.8">
       <c r="A44" s="2" t="s">
         <v>62</v>
       </c>
@@ -14844,7 +16236,7 @@
         <v>group1</v>
       </c>
     </row>
-    <row r="45" spans="1:16" ht="14.25" hidden="1">
+    <row r="45" spans="1:16" ht="13.8">
       <c r="A45" s="2" t="s">
         <v>62</v>
       </c>
@@ -14878,7 +16270,7 @@
         <v>group1</v>
       </c>
     </row>
-    <row r="46" spans="1:16" ht="14.25" hidden="1">
+    <row r="46" spans="1:16" ht="13.8">
       <c r="A46" s="6" t="s">
         <v>62</v>
       </c>
@@ -14917,7 +16309,7 @@
         <v>group1</v>
       </c>
     </row>
-    <row r="47" spans="1:16" ht="14.25" hidden="1">
+    <row r="47" spans="1:16" ht="13.8">
       <c r="A47" s="6" t="s">
         <v>62</v>
       </c>
@@ -14958,7 +16350,7 @@
         <v>group1</v>
       </c>
     </row>
-    <row r="48" spans="1:16" ht="14.25" hidden="1">
+    <row r="48" spans="1:16" ht="13.8">
       <c r="A48" s="6" t="s">
         <v>62</v>
       </c>
@@ -14999,7 +16391,7 @@
         <v>group1</v>
       </c>
     </row>
-    <row r="49" spans="1:14" ht="14.25" hidden="1">
+    <row r="49" spans="1:14" ht="13.8">
       <c r="A49" s="6" t="s">
         <v>62</v>
       </c>
@@ -15040,7 +16432,7 @@
         <v>group1</v>
       </c>
     </row>
-    <row r="50" spans="1:14" ht="14.25" hidden="1">
+    <row r="50" spans="1:14" ht="13.8">
       <c r="A50" s="6" t="s">
         <v>62</v>
       </c>
@@ -15081,7 +16473,7 @@
         <v>group1</v>
       </c>
     </row>
-    <row r="51" spans="1:14" ht="14.25" hidden="1">
+    <row r="51" spans="1:14" ht="13.8">
       <c r="A51" s="6" t="s">
         <v>62</v>
       </c>
@@ -15122,7 +16514,7 @@
         <v>group1</v>
       </c>
     </row>
-    <row r="52" spans="1:14" ht="14.25" hidden="1">
+    <row r="52" spans="1:14" ht="13.8">
       <c r="A52" s="6" t="s">
         <v>62</v>
       </c>
@@ -15163,7 +16555,7 @@
         <v>group1</v>
       </c>
     </row>
-    <row r="53" spans="1:14" ht="14.25" hidden="1">
+    <row r="53" spans="1:14" ht="13.8">
       <c r="A53" s="6" t="s">
         <v>62</v>
       </c>
@@ -15204,7 +16596,7 @@
         <v>group1</v>
       </c>
     </row>
-    <row r="54" spans="1:14" ht="14.25" hidden="1">
+    <row r="54" spans="1:14" ht="13.8">
       <c r="A54" s="6" t="s">
         <v>62</v>
       </c>
@@ -15245,7 +16637,7 @@
         <v>group1</v>
       </c>
     </row>
-    <row r="55" spans="1:14" ht="14.25" hidden="1">
+    <row r="55" spans="1:14" ht="13.8">
       <c r="A55" s="6" t="s">
         <v>62</v>
       </c>
@@ -15284,7 +16676,7 @@
         <v>group1</v>
       </c>
     </row>
-    <row r="56" spans="1:14" ht="14.25" hidden="1">
+    <row r="56" spans="1:14" ht="13.8">
       <c r="A56" s="2" t="s">
         <v>66</v>
       </c>
@@ -15318,7 +16710,7 @@
         <v>group3</v>
       </c>
     </row>
-    <row r="57" spans="1:14" ht="14.25" hidden="1">
+    <row r="57" spans="1:14" ht="13.8">
       <c r="A57" s="2" t="s">
         <v>66</v>
       </c>
@@ -15355,7 +16747,7 @@
         <v>group3</v>
       </c>
     </row>
-    <row r="58" spans="1:14" ht="14.25" hidden="1">
+    <row r="58" spans="1:14" ht="13.8">
       <c r="A58" s="2" t="s">
         <v>66</v>
       </c>
@@ -15392,7 +16784,7 @@
         <v>group3</v>
       </c>
     </row>
-    <row r="59" spans="1:14" ht="14.25" hidden="1">
+    <row r="59" spans="1:14" ht="13.8">
       <c r="A59" s="2" t="s">
         <v>66</v>
       </c>
@@ -15426,7 +16818,7 @@
         <v>group3</v>
       </c>
     </row>
-    <row r="60" spans="1:14" ht="14.25" hidden="1">
+    <row r="60" spans="1:14" ht="13.8">
       <c r="A60" s="6" t="s">
         <v>66</v>
       </c>
@@ -15465,7 +16857,7 @@
         <v>group3</v>
       </c>
     </row>
-    <row r="61" spans="1:14" ht="14.25" hidden="1">
+    <row r="61" spans="1:14" ht="13.8">
       <c r="A61" s="6" t="s">
         <v>66</v>
       </c>
@@ -15506,7 +16898,7 @@
         <v>group3</v>
       </c>
     </row>
-    <row r="62" spans="1:14" ht="14.25" hidden="1">
+    <row r="62" spans="1:14" ht="13.8">
       <c r="A62" s="6" t="s">
         <v>66</v>
       </c>
@@ -15547,7 +16939,7 @@
         <v>group3</v>
       </c>
     </row>
-    <row r="63" spans="1:14" ht="14.25" hidden="1">
+    <row r="63" spans="1:14" ht="13.8">
       <c r="A63" s="6" t="s">
         <v>66</v>
       </c>
@@ -15586,7 +16978,7 @@
         <v>group3</v>
       </c>
     </row>
-    <row r="64" spans="1:14" ht="14.25" hidden="1">
+    <row r="64" spans="1:14" ht="13.8">
       <c r="A64" s="2" t="s">
         <v>66</v>
       </c>
@@ -15620,7 +17012,7 @@
         <v>group3</v>
       </c>
     </row>
-    <row r="65" spans="1:14" ht="14.25" hidden="1">
+    <row r="65" spans="1:14" ht="13.8">
       <c r="A65" s="2" t="s">
         <v>66</v>
       </c>
@@ -15657,7 +17049,7 @@
         <v>group3</v>
       </c>
     </row>
-    <row r="66" spans="1:14" ht="14.25" hidden="1">
+    <row r="66" spans="1:14" ht="13.8">
       <c r="A66" s="2" t="s">
         <v>66</v>
       </c>
@@ -15694,7 +17086,7 @@
         <v>group3</v>
       </c>
     </row>
-    <row r="67" spans="1:14" ht="14.25" hidden="1">
+    <row r="67" spans="1:14" ht="13.8">
       <c r="A67" s="2" t="s">
         <v>66</v>
       </c>
@@ -15731,7 +17123,7 @@
         <v>group3</v>
       </c>
     </row>
-    <row r="68" spans="1:14" ht="14.25" hidden="1">
+    <row r="68" spans="1:14" ht="13.8">
       <c r="A68" s="2" t="s">
         <v>66</v>
       </c>
@@ -15765,7 +17157,7 @@
         <v>group3</v>
       </c>
     </row>
-    <row r="69" spans="1:14" ht="14.25">
+    <row r="69" spans="1:14" ht="13.8">
       <c r="A69" s="6" t="s">
         <v>72</v>
       </c>
@@ -15804,7 +17196,7 @@
         <v>group1</v>
       </c>
     </row>
-    <row r="70" spans="1:14" ht="14.25">
+    <row r="70" spans="1:14" ht="13.8">
       <c r="A70" s="6" t="s">
         <v>72</v>
       </c>
@@ -15845,7 +17237,7 @@
         <v>group1</v>
       </c>
     </row>
-    <row r="71" spans="1:14" ht="14.25">
+    <row r="71" spans="1:14" ht="13.8">
       <c r="A71" s="6" t="s">
         <v>72</v>
       </c>
@@ -15886,7 +17278,7 @@
         <v>group1</v>
       </c>
     </row>
-    <row r="72" spans="1:14" ht="14.25">
+    <row r="72" spans="1:14" ht="13.8">
       <c r="A72" s="6" t="s">
         <v>72</v>
       </c>
@@ -15925,7 +17317,7 @@
         <v>group1</v>
       </c>
     </row>
-    <row r="73" spans="1:14" ht="14.25" hidden="1">
+    <row r="73" spans="1:14" ht="13.8">
       <c r="A73" s="2" t="s">
         <v>72</v>
       </c>
@@ -15959,7 +17351,7 @@
         <v>group1</v>
       </c>
     </row>
-    <row r="74" spans="1:14" ht="14.25" hidden="1">
+    <row r="74" spans="1:14" ht="13.8">
       <c r="A74" s="2" t="s">
         <v>72</v>
       </c>
@@ -15996,7 +17388,7 @@
         <v>group1</v>
       </c>
     </row>
-    <row r="75" spans="1:14" ht="14.25" hidden="1">
+    <row r="75" spans="1:14" ht="13.8">
       <c r="A75" s="2" t="s">
         <v>72</v>
       </c>
@@ -16033,7 +17425,7 @@
         <v>group1</v>
       </c>
     </row>
-    <row r="76" spans="1:14" ht="14.25" hidden="1">
+    <row r="76" spans="1:14" ht="13.8">
       <c r="A76" s="2" t="s">
         <v>72</v>
       </c>
@@ -16070,7 +17462,7 @@
         <v>group1</v>
       </c>
     </row>
-    <row r="77" spans="1:14" ht="14.25" hidden="1">
+    <row r="77" spans="1:14" ht="13.8">
       <c r="A77" s="2" t="s">
         <v>72</v>
       </c>
@@ -16107,7 +17499,7 @@
         <v>group1</v>
       </c>
     </row>
-    <row r="78" spans="1:14" ht="14.25" hidden="1">
+    <row r="78" spans="1:14" ht="13.8">
       <c r="A78" s="2" t="s">
         <v>72</v>
       </c>
@@ -16141,7 +17533,7 @@
         <v>group1</v>
       </c>
     </row>
-    <row r="79" spans="1:14" ht="14.25" hidden="1">
+    <row r="79" spans="1:14" ht="13.8">
       <c r="A79" s="2" t="s">
         <v>72</v>
       </c>
@@ -16175,7 +17567,7 @@
         <v>group1</v>
       </c>
     </row>
-    <row r="80" spans="1:14" ht="14.25" hidden="1">
+    <row r="80" spans="1:14" ht="13.8">
       <c r="A80" s="6" t="s">
         <v>72</v>
       </c>
@@ -16216,7 +17608,7 @@
         <v>group1</v>
       </c>
     </row>
-    <row r="81" spans="1:14" ht="14.25" hidden="1">
+    <row r="81" spans="1:14" ht="13.8">
       <c r="A81" s="6" t="s">
         <v>72</v>
       </c>
@@ -16257,7 +17649,7 @@
         <v>group1</v>
       </c>
     </row>
-    <row r="82" spans="1:14" ht="14.25" hidden="1">
+    <row r="82" spans="1:14" ht="13.8">
       <c r="A82" s="6" t="s">
         <v>72</v>
       </c>
@@ -16296,7 +17688,7 @@
         <v>group1</v>
       </c>
     </row>
-    <row r="83" spans="1:14" ht="14.25">
+    <row r="83" spans="1:14" ht="13.8">
       <c r="A83" s="2" t="s">
         <v>81</v>
       </c>
@@ -16330,7 +17722,7 @@
         <v>group1</v>
       </c>
     </row>
-    <row r="84" spans="1:14" ht="14.25">
+    <row r="84" spans="1:14" ht="13.8">
       <c r="A84" s="2" t="s">
         <v>81</v>
       </c>
@@ -16367,7 +17759,7 @@
         <v>group1</v>
       </c>
     </row>
-    <row r="85" spans="1:14" ht="14.25">
+    <row r="85" spans="1:14" ht="13.8">
       <c r="A85" s="2" t="s">
         <v>81</v>
       </c>
@@ -16404,7 +17796,7 @@
         <v>group1</v>
       </c>
     </row>
-    <row r="86" spans="1:14" ht="14.25">
+    <row r="86" spans="1:14" ht="13.8">
       <c r="A86" s="2" t="s">
         <v>81</v>
       </c>
@@ -16441,7 +17833,7 @@
         <v>group1</v>
       </c>
     </row>
-    <row r="87" spans="1:14" ht="14.25">
+    <row r="87" spans="1:14" ht="13.8">
       <c r="A87" s="2" t="s">
         <v>81</v>
       </c>
@@ -16475,7 +17867,7 @@
         <v>group1</v>
       </c>
     </row>
-    <row r="88" spans="1:14" ht="14.25" hidden="1">
+    <row r="88" spans="1:14" ht="13.8">
       <c r="A88" s="6" t="s">
         <v>81</v>
       </c>
@@ -16514,7 +17906,7 @@
         <v>group1</v>
       </c>
     </row>
-    <row r="89" spans="1:14" ht="14.25" hidden="1">
+    <row r="89" spans="1:14" ht="13.8">
       <c r="A89" s="6" t="s">
         <v>81</v>
       </c>
@@ -16555,7 +17947,7 @@
         <v>group1</v>
       </c>
     </row>
-    <row r="90" spans="1:14" ht="14.25" hidden="1">
+    <row r="90" spans="1:14" ht="13.8">
       <c r="A90" s="6" t="s">
         <v>81</v>
       </c>
@@ -16596,7 +17988,7 @@
         <v>group1</v>
       </c>
     </row>
-    <row r="91" spans="1:14" ht="14.25" hidden="1">
+    <row r="91" spans="1:14" ht="13.8">
       <c r="A91" s="6" t="s">
         <v>81</v>
       </c>
@@ -16637,7 +18029,7 @@
         <v>group1</v>
       </c>
     </row>
-    <row r="92" spans="1:14" ht="14.25" hidden="1">
+    <row r="92" spans="1:14" ht="13.8">
       <c r="A92" s="6" t="s">
         <v>81</v>
       </c>
@@ -16678,7 +18070,7 @@
         <v>group1</v>
       </c>
     </row>
-    <row r="93" spans="1:14" ht="14.25" hidden="1">
+    <row r="93" spans="1:14" ht="13.8">
       <c r="A93" s="6" t="s">
         <v>81</v>
       </c>
@@ -16719,7 +18111,7 @@
         <v>group1</v>
       </c>
     </row>
-    <row r="94" spans="1:14" ht="14.25" hidden="1">
+    <row r="94" spans="1:14" ht="13.8">
       <c r="A94" s="6" t="s">
         <v>81</v>
       </c>
@@ -16760,7 +18152,7 @@
         <v>group1</v>
       </c>
     </row>
-    <row r="95" spans="1:14" ht="14.25" hidden="1">
+    <row r="95" spans="1:14" ht="13.8">
       <c r="A95" s="6" t="s">
         <v>81</v>
       </c>
@@ -16801,7 +18193,7 @@
         <v>group1</v>
       </c>
     </row>
-    <row r="96" spans="1:14" ht="14.25" hidden="1">
+    <row r="96" spans="1:14" ht="13.8">
       <c r="A96" s="6" t="s">
         <v>81</v>
       </c>
@@ -16840,7 +18232,7 @@
         <v>group1</v>
       </c>
     </row>
-    <row r="97" spans="1:14" ht="14.25" hidden="1">
+    <row r="97" spans="1:14" ht="13.8">
       <c r="A97" s="2" t="s">
         <v>81</v>
       </c>
@@ -16874,7 +18266,7 @@
         <v>group1</v>
       </c>
     </row>
-    <row r="98" spans="1:14" ht="14.25" hidden="1">
+    <row r="98" spans="1:14" ht="13.8">
       <c r="A98" s="2" t="s">
         <v>81</v>
       </c>
@@ -16911,7 +18303,7 @@
         <v>group1</v>
       </c>
     </row>
-    <row r="99" spans="1:14" ht="14.25" hidden="1">
+    <row r="99" spans="1:14" ht="13.8">
       <c r="A99" s="2" t="s">
         <v>81</v>
       </c>
@@ -16948,7 +18340,7 @@
         <v>group1</v>
       </c>
     </row>
-    <row r="100" spans="1:14" ht="14.25" hidden="1">
+    <row r="100" spans="1:14" ht="13.8">
       <c r="A100" s="2" t="s">
         <v>81</v>
       </c>
@@ -16982,7 +18374,7 @@
         <v>group1</v>
       </c>
     </row>
-    <row r="101" spans="1:14" ht="14.25">
+    <row r="101" spans="1:14" ht="13.8">
       <c r="A101" s="6" t="s">
         <v>82</v>
       </c>
@@ -17021,7 +18413,7 @@
         <v>group1</v>
       </c>
     </row>
-    <row r="102" spans="1:14" ht="14.25">
+    <row r="102" spans="1:14" ht="13.8">
       <c r="A102" s="6" t="s">
         <v>82</v>
       </c>
@@ -17062,7 +18454,7 @@
         <v>group1</v>
       </c>
     </row>
-    <row r="103" spans="1:14" ht="14.25">
+    <row r="103" spans="1:14" ht="13.8">
       <c r="A103" s="6" t="s">
         <v>82</v>
       </c>
@@ -17103,7 +18495,7 @@
         <v>group1</v>
       </c>
     </row>
-    <row r="104" spans="1:14" ht="14.25">
+    <row r="104" spans="1:14" ht="13.8">
       <c r="A104" s="6" t="s">
         <v>82</v>
       </c>
@@ -17144,7 +18536,7 @@
         <v>group1</v>
       </c>
     </row>
-    <row r="105" spans="1:14" ht="14.25">
+    <row r="105" spans="1:14" ht="13.8">
       <c r="A105" s="6" t="s">
         <v>82</v>
       </c>
@@ -17185,7 +18577,7 @@
         <v>group1</v>
       </c>
     </row>
-    <row r="106" spans="1:14" ht="14.25">
+    <row r="106" spans="1:14" ht="13.8">
       <c r="A106" s="6" t="s">
         <v>82</v>
       </c>
@@ -17224,7 +18616,7 @@
         <v>group1</v>
       </c>
     </row>
-    <row r="107" spans="1:14" ht="14.25" hidden="1">
+    <row r="107" spans="1:14" ht="13.8">
       <c r="A107" s="2" t="s">
         <v>82</v>
       </c>
@@ -17258,7 +18650,7 @@
         <v>group1</v>
       </c>
     </row>
-    <row r="108" spans="1:14" ht="14.25" hidden="1">
+    <row r="108" spans="1:14" ht="13.8">
       <c r="A108" s="2" t="s">
         <v>82</v>
       </c>
@@ -17295,7 +18687,7 @@
         <v>group1</v>
       </c>
     </row>
-    <row r="109" spans="1:14" ht="14.25" hidden="1">
+    <row r="109" spans="1:14" ht="13.8">
       <c r="A109" s="2" t="s">
         <v>82</v>
       </c>
@@ -17332,7 +18724,7 @@
         <v>group1</v>
       </c>
     </row>
-    <row r="110" spans="1:14" ht="14.25" hidden="1">
+    <row r="110" spans="1:14" ht="13.8">
       <c r="A110" s="2" t="s">
         <v>82</v>
       </c>
@@ -17369,7 +18761,7 @@
         <v>group1</v>
       </c>
     </row>
-    <row r="111" spans="1:14" ht="14.25" hidden="1">
+    <row r="111" spans="1:14" ht="13.8">
       <c r="A111" s="2" t="s">
         <v>82</v>
       </c>
@@ -17406,7 +18798,7 @@
         <v>group1</v>
       </c>
     </row>
-    <row r="112" spans="1:14" ht="14.25" hidden="1">
+    <row r="112" spans="1:14" ht="13.8">
       <c r="A112" s="2" t="s">
         <v>82</v>
       </c>
@@ -17443,7 +18835,7 @@
         <v>group1</v>
       </c>
     </row>
-    <row r="113" spans="1:14" ht="14.25" hidden="1">
+    <row r="113" spans="1:14" ht="13.8">
       <c r="A113" s="2" t="s">
         <v>82</v>
       </c>
@@ -17477,7 +18869,7 @@
         <v>group1</v>
       </c>
     </row>
-    <row r="114" spans="1:14" ht="14.25" hidden="1">
+    <row r="114" spans="1:14" ht="13.8">
       <c r="A114" s="6" t="s">
         <v>82</v>
       </c>
@@ -17516,7 +18908,7 @@
         <v>group1</v>
       </c>
     </row>
-    <row r="115" spans="1:14" ht="14.25" hidden="1">
+    <row r="115" spans="1:14" ht="13.8">
       <c r="A115" s="6" t="s">
         <v>82</v>
       </c>
@@ -17557,7 +18949,7 @@
         <v>group1</v>
       </c>
     </row>
-    <row r="116" spans="1:14" ht="14.25" hidden="1">
+    <row r="116" spans="1:14" ht="13.8">
       <c r="A116" s="6" t="s">
         <v>82</v>
       </c>
@@ -17596,7 +18988,7 @@
         <v>group1</v>
       </c>
     </row>
-    <row r="117" spans="1:14" ht="14.25">
+    <row r="117" spans="1:14" ht="13.8">
       <c r="A117" s="2" t="s">
         <v>85</v>
       </c>
@@ -17630,7 +19022,7 @@
         <v>group1</v>
       </c>
     </row>
-    <row r="118" spans="1:14" ht="14.25">
+    <row r="118" spans="1:14" ht="13.8">
       <c r="A118" s="2" t="s">
         <v>85</v>
       </c>
@@ -17667,7 +19059,7 @@
         <v>group1</v>
       </c>
     </row>
-    <row r="119" spans="1:14" ht="14.25">
+    <row r="119" spans="1:14" ht="13.8">
       <c r="A119" s="2" t="s">
         <v>85</v>
       </c>
@@ -17704,7 +19096,7 @@
         <v>group1</v>
       </c>
     </row>
-    <row r="120" spans="1:14" ht="14.25">
+    <row r="120" spans="1:14" ht="13.8">
       <c r="A120" s="2" t="s">
         <v>85</v>
       </c>
@@ -17738,7 +19130,7 @@
         <v>group1</v>
       </c>
     </row>
-    <row r="121" spans="1:14" ht="14.25" hidden="1">
+    <row r="121" spans="1:14" ht="13.8">
       <c r="A121" s="6" t="s">
         <v>85</v>
       </c>
@@ -17777,7 +19169,7 @@
         <v>group1</v>
       </c>
     </row>
-    <row r="122" spans="1:14" ht="14.25" hidden="1">
+    <row r="122" spans="1:14" ht="13.8">
       <c r="A122" s="6" t="s">
         <v>85</v>
       </c>
@@ -17818,7 +19210,7 @@
         <v>group1</v>
       </c>
     </row>
-    <row r="123" spans="1:14" ht="14.25" hidden="1">
+    <row r="123" spans="1:14" ht="13.8">
       <c r="A123" s="6" t="s">
         <v>85</v>
       </c>
@@ -17859,7 +19251,7 @@
         <v>group1</v>
       </c>
     </row>
-    <row r="124" spans="1:14" ht="14.25" hidden="1">
+    <row r="124" spans="1:14" ht="13.8">
       <c r="A124" s="6" t="s">
         <v>85</v>
       </c>
@@ -17900,7 +19292,7 @@
         <v>group1</v>
       </c>
     </row>
-    <row r="125" spans="1:14" ht="14.25" hidden="1">
+    <row r="125" spans="1:14" ht="13.8">
       <c r="A125" s="6" t="s">
         <v>85</v>
       </c>
@@ -17939,7 +19331,7 @@
         <v>group1</v>
       </c>
     </row>
-    <row r="126" spans="1:14" ht="14.25" hidden="1">
+    <row r="126" spans="1:14" ht="13.8">
       <c r="A126" s="2" t="s">
         <v>85</v>
       </c>
@@ -17973,7 +19365,7 @@
         <v>group1</v>
       </c>
     </row>
-    <row r="127" spans="1:14" ht="14.25" hidden="1">
+    <row r="127" spans="1:14" ht="13.8">
       <c r="A127" s="2" t="s">
         <v>85</v>
       </c>
@@ -18010,7 +19402,7 @@
         <v>group1</v>
       </c>
     </row>
-    <row r="128" spans="1:14" ht="14.25" hidden="1">
+    <row r="128" spans="1:14" ht="13.8">
       <c r="A128" s="2" t="s">
         <v>85</v>
       </c>
@@ -18047,7 +19439,7 @@
         <v>group1</v>
       </c>
     </row>
-    <row r="129" spans="1:14" ht="14.25" hidden="1">
+    <row r="129" spans="1:14" ht="13.8">
       <c r="A129" s="2" t="s">
         <v>85</v>
       </c>
@@ -18084,7 +19476,7 @@
         <v>group1</v>
       </c>
     </row>
-    <row r="130" spans="1:14" ht="14.25" hidden="1">
+    <row r="130" spans="1:14" ht="13.8">
       <c r="A130" s="2" t="s">
         <v>85</v>
       </c>
@@ -18118,7 +19510,7 @@
         <v>group1</v>
       </c>
     </row>
-    <row r="131" spans="1:14" ht="14.25">
+    <row r="131" spans="1:14" ht="13.8">
       <c r="A131" s="6" t="s">
         <v>88</v>
       </c>
@@ -18157,7 +19549,7 @@
         <v>group1</v>
       </c>
     </row>
-    <row r="132" spans="1:14" ht="14.25">
+    <row r="132" spans="1:14" ht="13.8">
       <c r="A132" s="6" t="s">
         <v>88</v>
       </c>
@@ -18198,7 +19590,7 @@
         <v>group1</v>
       </c>
     </row>
-    <row r="133" spans="1:14" ht="14.25">
+    <row r="133" spans="1:14" ht="13.8">
       <c r="A133" s="6" t="s">
         <v>88</v>
       </c>
@@ -18239,7 +19631,7 @@
         <v>group1</v>
       </c>
     </row>
-    <row r="134" spans="1:14" ht="14.25">
+    <row r="134" spans="1:14" ht="13.8">
       <c r="A134" s="6" t="s">
         <v>88</v>
       </c>
@@ -18280,7 +19672,7 @@
         <v>group1</v>
       </c>
     </row>
-    <row r="135" spans="1:14" ht="14.25">
+    <row r="135" spans="1:14" ht="13.8">
       <c r="A135" s="6" t="s">
         <v>88</v>
       </c>
@@ -18319,7 +19711,7 @@
         <v>group1</v>
       </c>
     </row>
-    <row r="136" spans="1:14" ht="14.25" hidden="1">
+    <row r="136" spans="1:14" ht="13.8">
       <c r="A136" s="2" t="s">
         <v>88</v>
       </c>
@@ -18353,7 +19745,7 @@
         <v>group1</v>
       </c>
     </row>
-    <row r="137" spans="1:14" ht="14.25" hidden="1">
+    <row r="137" spans="1:14" ht="13.8">
       <c r="A137" s="2" t="s">
         <v>88</v>
       </c>
@@ -18390,7 +19782,7 @@
         <v>group1</v>
       </c>
     </row>
-    <row r="138" spans="1:14" ht="14.25" hidden="1">
+    <row r="138" spans="1:14" ht="13.8">
       <c r="A138" s="2" t="s">
         <v>88</v>
       </c>
@@ -18427,7 +19819,7 @@
         <v>group1</v>
       </c>
     </row>
-    <row r="139" spans="1:14" ht="14.25" hidden="1">
+    <row r="139" spans="1:14" ht="13.8">
       <c r="A139" s="2" t="s">
         <v>88</v>
       </c>
@@ -18464,7 +19856,7 @@
         <v>group1</v>
       </c>
     </row>
-    <row r="140" spans="1:14" ht="14.25" hidden="1">
+    <row r="140" spans="1:14" ht="13.8">
       <c r="A140" s="2" t="s">
         <v>88</v>
       </c>
@@ -18501,7 +19893,7 @@
         <v>group1</v>
       </c>
     </row>
-    <row r="141" spans="1:14" ht="14.25" hidden="1">
+    <row r="141" spans="1:14" ht="13.8">
       <c r="A141" s="2" t="s">
         <v>88</v>
       </c>
@@ -18535,7 +19927,7 @@
         <v>group1</v>
       </c>
     </row>
-    <row r="142" spans="1:14" ht="14.25" hidden="1">
+    <row r="142" spans="1:14" ht="13.8">
       <c r="A142" s="6" t="s">
         <v>88</v>
       </c>
@@ -18574,7 +19966,7 @@
         <v>group1</v>
       </c>
     </row>
-    <row r="143" spans="1:14" ht="14.25" hidden="1">
+    <row r="143" spans="1:14" ht="13.8">
       <c r="A143" s="6" t="s">
         <v>88</v>
       </c>
@@ -18615,7 +20007,7 @@
         <v>group1</v>
       </c>
     </row>
-    <row r="144" spans="1:14" ht="14.25" hidden="1">
+    <row r="144" spans="1:14" ht="13.8">
       <c r="A144" s="6" t="s">
         <v>88</v>
       </c>
@@ -18654,7 +20046,7 @@
         <v>group1</v>
       </c>
     </row>
-    <row r="145" spans="1:14" ht="14.25" hidden="1">
+    <row r="145" spans="1:14" ht="13.8">
       <c r="A145" s="2" t="s">
         <v>90</v>
       </c>
@@ -18688,7 +20080,7 @@
         <v>group2</v>
       </c>
     </row>
-    <row r="146" spans="1:14" ht="14.25" hidden="1">
+    <row r="146" spans="1:14" ht="13.8">
       <c r="A146" s="2" t="s">
         <v>90</v>
       </c>
@@ -18725,7 +20117,7 @@
         <v>group2</v>
       </c>
     </row>
-    <row r="147" spans="1:14" ht="14.25" hidden="1">
+    <row r="147" spans="1:14" ht="13.8">
       <c r="A147" s="2" t="s">
         <v>90</v>
       </c>
@@ -18762,7 +20154,7 @@
         <v>group2</v>
       </c>
     </row>
-    <row r="148" spans="1:14" ht="14.25" hidden="1">
+    <row r="148" spans="1:14" ht="13.8">
       <c r="A148" s="2" t="s">
         <v>90</v>
       </c>
@@ -18799,7 +20191,7 @@
         <v>group2</v>
       </c>
     </row>
-    <row r="149" spans="1:14" ht="14.25" hidden="1">
+    <row r="149" spans="1:14" ht="13.8">
       <c r="A149" s="2" t="s">
         <v>90</v>
       </c>
@@ -18833,7 +20225,7 @@
         <v>group2</v>
       </c>
     </row>
-    <row r="150" spans="1:14" ht="14.25" hidden="1">
+    <row r="150" spans="1:14" ht="13.8">
       <c r="A150" s="6" t="s">
         <v>90</v>
       </c>
@@ -18872,7 +20264,7 @@
         <v>group2</v>
       </c>
     </row>
-    <row r="151" spans="1:14" ht="14.25" hidden="1">
+    <row r="151" spans="1:14" ht="13.8">
       <c r="A151" s="6" t="s">
         <v>90</v>
       </c>
@@ -18913,7 +20305,7 @@
         <v>group2</v>
       </c>
     </row>
-    <row r="152" spans="1:14" ht="14.25" hidden="1">
+    <row r="152" spans="1:14" ht="13.8">
       <c r="A152" s="6" t="s">
         <v>90</v>
       </c>
@@ -18954,7 +20346,7 @@
         <v>group2</v>
       </c>
     </row>
-    <row r="153" spans="1:14" ht="14.25" hidden="1">
+    <row r="153" spans="1:14" ht="13.8">
       <c r="A153" s="6" t="s">
         <v>90</v>
       </c>
@@ -18993,7 +20385,7 @@
         <v>group2</v>
       </c>
     </row>
-    <row r="154" spans="1:14" ht="14.25" hidden="1">
+    <row r="154" spans="1:14" ht="13.8">
       <c r="A154" s="2" t="s">
         <v>90</v>
       </c>
@@ -19027,7 +20419,7 @@
         <v>group2</v>
       </c>
     </row>
-    <row r="155" spans="1:14" ht="14.25" hidden="1">
+    <row r="155" spans="1:14" ht="13.8">
       <c r="A155" s="2" t="s">
         <v>90</v>
       </c>
@@ -19064,7 +20456,7 @@
         <v>group2</v>
       </c>
     </row>
-    <row r="156" spans="1:14" ht="14.25" hidden="1">
+    <row r="156" spans="1:14" ht="13.8">
       <c r="A156" s="2" t="s">
         <v>90</v>
       </c>
@@ -19101,7 +20493,7 @@
         <v>group2</v>
       </c>
     </row>
-    <row r="157" spans="1:14" ht="14.25" hidden="1">
+    <row r="157" spans="1:14" ht="13.8">
       <c r="A157" s="2" t="s">
         <v>90</v>
       </c>
@@ -19138,7 +20530,7 @@
         <v>group2</v>
       </c>
     </row>
-    <row r="158" spans="1:14" ht="14.25" hidden="1">
+    <row r="158" spans="1:14" ht="13.8">
       <c r="A158" s="2" t="s">
         <v>90</v>
       </c>
@@ -19175,7 +20567,7 @@
         <v>group2</v>
       </c>
     </row>
-    <row r="159" spans="1:14" ht="14.25" hidden="1">
+    <row r="159" spans="1:14" ht="13.8">
       <c r="A159" s="2" t="s">
         <v>90</v>
       </c>
@@ -19209,7 +20601,7 @@
         <v>group2</v>
       </c>
     </row>
-    <row r="160" spans="1:14" ht="14.25" hidden="1">
+    <row r="160" spans="1:14" ht="13.8">
       <c r="A160" s="6" t="s">
         <v>91</v>
       </c>
@@ -19248,7 +20640,7 @@
         <v>group2</v>
       </c>
     </row>
-    <row r="161" spans="1:14" ht="14.25" hidden="1">
+    <row r="161" spans="1:14" ht="13.8">
       <c r="A161" s="6" t="s">
         <v>91</v>
       </c>
@@ -19289,7 +20681,7 @@
         <v>group2</v>
       </c>
     </row>
-    <row r="162" spans="1:14" ht="14.25" hidden="1">
+    <row r="162" spans="1:14" ht="13.8">
       <c r="A162" s="6" t="s">
         <v>91</v>
       </c>
@@ -19300,7 +20692,7 @@
         <v>1</v>
       </c>
       <c r="D162" s="6" t="str">
-        <f t="shared" ref="D162:D193" si="10">_xlfn.TEXTJOIN("-",,B162,C162)</f>
+        <f t="shared" ref="D162:D177" si="10">_xlfn.TEXTJOIN("-",,B162,C162)</f>
         <v>P07-1</v>
       </c>
       <c r="E162" s="9" t="str">
@@ -19330,7 +20722,7 @@
         <v>group2</v>
       </c>
     </row>
-    <row r="163" spans="1:14" ht="14.25" hidden="1">
+    <row r="163" spans="1:14" ht="13.8">
       <c r="A163" s="6" t="s">
         <v>91</v>
       </c>
@@ -19371,7 +20763,7 @@
         <v>group2</v>
       </c>
     </row>
-    <row r="164" spans="1:14" ht="14.25" hidden="1">
+    <row r="164" spans="1:14" ht="13.8">
       <c r="A164" s="6" t="s">
         <v>91</v>
       </c>
@@ -19410,7 +20802,7 @@
         <v>group2</v>
       </c>
     </row>
-    <row r="165" spans="1:14" ht="14.25" hidden="1">
+    <row r="165" spans="1:14" ht="13.8">
       <c r="A165" s="2" t="s">
         <v>91</v>
       </c>
@@ -19444,7 +20836,7 @@
         <v>group2</v>
       </c>
     </row>
-    <row r="166" spans="1:14" ht="14.25" hidden="1">
+    <row r="166" spans="1:14" ht="13.8">
       <c r="A166" s="2" t="s">
         <v>91</v>
       </c>
@@ -19481,7 +20873,7 @@
         <v>group2</v>
       </c>
     </row>
-    <row r="167" spans="1:14" ht="14.25" hidden="1">
+    <row r="167" spans="1:14" ht="13.8">
       <c r="A167" s="2" t="s">
         <v>91</v>
       </c>
@@ -19518,7 +20910,7 @@
         <v>group2</v>
       </c>
     </row>
-    <row r="168" spans="1:14" ht="14.25" hidden="1">
+    <row r="168" spans="1:14" ht="13.8">
       <c r="A168" s="2" t="s">
         <v>91</v>
       </c>
@@ -19555,7 +20947,7 @@
         <v>group2</v>
       </c>
     </row>
-    <row r="169" spans="1:14" ht="14.25" hidden="1">
+    <row r="169" spans="1:14" ht="13.8">
       <c r="A169" s="2" t="s">
         <v>91</v>
       </c>
@@ -19592,7 +20984,7 @@
         <v>group2</v>
       </c>
     </row>
-    <row r="170" spans="1:14" ht="14.25" hidden="1">
+    <row r="170" spans="1:14" ht="13.8">
       <c r="A170" s="2" t="s">
         <v>91</v>
       </c>
@@ -19629,7 +21021,7 @@
         <v>group2</v>
       </c>
     </row>
-    <row r="171" spans="1:14" ht="14.25" hidden="1">
+    <row r="171" spans="1:14" ht="13.8">
       <c r="A171" s="2" t="s">
         <v>91</v>
       </c>
@@ -19663,7 +21055,7 @@
         <v>group2</v>
       </c>
     </row>
-    <row r="172" spans="1:14" ht="14.25" hidden="1">
+    <row r="172" spans="1:14" ht="13.8">
       <c r="A172" s="6" t="s">
         <v>91</v>
       </c>
@@ -19702,7 +21094,7 @@
         <v>group2</v>
       </c>
     </row>
-    <row r="173" spans="1:14" ht="14.25" hidden="1">
+    <row r="173" spans="1:14" ht="13.8">
       <c r="A173" s="6" t="s">
         <v>91</v>
       </c>
@@ -19743,7 +21135,7 @@
         <v>group2</v>
       </c>
     </row>
-    <row r="174" spans="1:14" ht="14.25" hidden="1">
+    <row r="174" spans="1:14" ht="13.8">
       <c r="A174" s="6" t="s">
         <v>91</v>
       </c>
@@ -19784,7 +21176,7 @@
         <v>group2</v>
       </c>
     </row>
-    <row r="175" spans="1:14" ht="14.25" hidden="1">
+    <row r="175" spans="1:14" ht="13.8">
       <c r="A175" s="6" t="s">
         <v>91</v>
       </c>
@@ -19825,7 +21217,7 @@
         <v>group2</v>
       </c>
     </row>
-    <row r="176" spans="1:14" ht="14.25" hidden="1">
+    <row r="176" spans="1:14" ht="13.8">
       <c r="A176" s="6" t="s">
         <v>91</v>
       </c>
@@ -19866,7 +21258,7 @@
         <v>group2</v>
       </c>
     </row>
-    <row r="177" spans="1:14" ht="14.25" hidden="1">
+    <row r="177" spans="1:14" ht="13.8">
       <c r="A177" s="6" t="s">
         <v>91</v>
       </c>
@@ -19913,18 +21305,7 @@
       <c r="L179" s="49"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:Q177">
-    <filterColumn colId="2">
-      <filters>
-        <filter val="1"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="13">
-      <filters>
-        <filter val="group1"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:Q177"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -19934,83 +21315,83 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A6" workbookViewId="0">
       <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="2" max="2" width="11.7109375" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" style="43" customWidth="1"/>
-    <col min="4" max="5" width="11.7109375" customWidth="1"/>
-    <col min="6" max="6" width="19.28515625" customWidth="1"/>
-    <col min="7" max="8" width="12.7109375" customWidth="1"/>
-    <col min="9" max="9" width="11.7109375" customWidth="1"/>
-    <col min="10" max="10" width="19.28515625" customWidth="1"/>
-    <col min="11" max="11" width="11.5703125" customWidth="1"/>
-    <col min="12" max="12" width="10.28515625" customWidth="1"/>
-    <col min="13" max="13" width="19.28515625" customWidth="1"/>
-    <col min="14" max="15" width="11.5703125" customWidth="1"/>
-    <col min="16" max="16" width="11.140625" customWidth="1"/>
-    <col min="17" max="17" width="19.28515625" customWidth="1"/>
-    <col min="18" max="18" width="11.5703125" customWidth="1"/>
-    <col min="19" max="19" width="10.5703125" customWidth="1"/>
-    <col min="20" max="20" width="19.28515625" customWidth="1"/>
-    <col min="21" max="21" width="11.5703125" customWidth="1"/>
-    <col min="22" max="22" width="10.7109375" customWidth="1"/>
-    <col min="23" max="23" width="19.28515625" customWidth="1"/>
-    <col min="24" max="25" width="13.7109375" customWidth="1"/>
-    <col min="26" max="26" width="19.28515625" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" style="43" customWidth="1"/>
+    <col min="4" max="5" width="11.6640625" customWidth="1"/>
+    <col min="6" max="6" width="19.33203125" customWidth="1"/>
+    <col min="7" max="8" width="12.6640625" customWidth="1"/>
+    <col min="9" max="9" width="11.6640625" customWidth="1"/>
+    <col min="10" max="10" width="19.33203125" customWidth="1"/>
+    <col min="11" max="11" width="11.5546875" customWidth="1"/>
+    <col min="12" max="12" width="10.33203125" customWidth="1"/>
+    <col min="13" max="13" width="19.33203125" customWidth="1"/>
+    <col min="14" max="15" width="11.5546875" customWidth="1"/>
+    <col min="16" max="16" width="11.109375" customWidth="1"/>
+    <col min="17" max="17" width="19.33203125" customWidth="1"/>
+    <col min="18" max="18" width="11.5546875" customWidth="1"/>
+    <col min="19" max="19" width="10.5546875" customWidth="1"/>
+    <col min="20" max="20" width="19.33203125" customWidth="1"/>
+    <col min="21" max="21" width="11.5546875" customWidth="1"/>
+    <col min="22" max="22" width="10.6640625" customWidth="1"/>
+    <col min="23" max="23" width="19.33203125" customWidth="1"/>
+    <col min="24" max="25" width="13.6640625" customWidth="1"/>
+    <col min="26" max="26" width="19.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="57" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="51" t="s">
+      <c r="B1" s="54" t="s">
         <v>23</v>
       </c>
       <c r="C1" s="42"/>
       <c r="D1" s="18"/>
-      <c r="E1" s="51" t="s">
+      <c r="E1" s="54" t="s">
         <v>109</v>
       </c>
-      <c r="F1" s="52"/>
-      <c r="G1" s="52"/>
-      <c r="I1" s="51" t="s">
+      <c r="F1" s="55"/>
+      <c r="G1" s="55"/>
+      <c r="I1" s="54" t="s">
         <v>110</v>
       </c>
-      <c r="J1" s="52"/>
-      <c r="K1" s="52"/>
-      <c r="L1" s="53" t="s">
+      <c r="J1" s="55"/>
+      <c r="K1" s="55"/>
+      <c r="L1" s="56" t="s">
         <v>111</v>
       </c>
-      <c r="M1" s="52"/>
-      <c r="N1" s="52"/>
-      <c r="P1" s="51" t="s">
+      <c r="M1" s="55"/>
+      <c r="N1" s="55"/>
+      <c r="P1" s="54" t="s">
         <v>112</v>
       </c>
-      <c r="Q1" s="52"/>
-      <c r="R1" s="52"/>
-      <c r="S1" s="53" t="s">
+      <c r="Q1" s="55"/>
+      <c r="R1" s="55"/>
+      <c r="S1" s="56" t="s">
         <v>113</v>
       </c>
-      <c r="T1" s="52"/>
-      <c r="U1" s="52"/>
-      <c r="V1" s="53" t="s">
+      <c r="T1" s="55"/>
+      <c r="U1" s="55"/>
+      <c r="V1" s="56" t="s">
         <v>114</v>
       </c>
-      <c r="W1" s="52"/>
-      <c r="X1" s="52"/>
-      <c r="Y1" s="53" t="s">
+      <c r="W1" s="55"/>
+      <c r="X1" s="55"/>
+      <c r="Y1" s="56" t="s">
         <v>115</v>
       </c>
-      <c r="Z1" s="52"/>
-      <c r="AA1" s="52"/>
+      <c r="Z1" s="55"/>
+      <c r="AA1" s="55"/>
     </row>
     <row r="2" spans="1:27" ht="15.75" customHeight="1">
-      <c r="A2" s="52"/>
-      <c r="B2" s="52"/>
+      <c r="A2" s="55"/>
+      <c r="B2" s="55"/>
       <c r="C2" s="31" t="s">
         <v>195</v>
       </c>
@@ -21391,7 +22772,7 @@
       <c r="G36" s="7"/>
       <c r="H36" s="7"/>
     </row>
-    <row r="37" spans="1:8" ht="12.75">
+    <row r="37" spans="1:8" ht="13.2">
       <c r="A37" s="2"/>
       <c r="B37" s="2"/>
       <c r="C37" s="44"/>
@@ -21401,7 +22782,7 @@
       <c r="G37" s="7"/>
       <c r="H37" s="7"/>
     </row>
-    <row r="38" spans="1:8" ht="12.75">
+    <row r="38" spans="1:8" ht="13.2">
       <c r="A38" s="2"/>
       <c r="B38" s="2"/>
       <c r="C38" s="44"/>
@@ -21411,7 +22792,7 @@
       <c r="G38" s="7"/>
       <c r="H38" s="7"/>
     </row>
-    <row r="39" spans="1:8" ht="12.75">
+    <row r="39" spans="1:8" ht="13.2">
       <c r="A39" s="2"/>
       <c r="B39" s="2"/>
       <c r="C39" s="44"/>
@@ -21421,7 +22802,7 @@
       <c r="G39" s="7"/>
       <c r="H39" s="7"/>
     </row>
-    <row r="40" spans="1:8" ht="12.75">
+    <row r="40" spans="1:8" ht="13.2">
       <c r="A40" s="2"/>
       <c r="B40" s="2"/>
       <c r="C40" s="44"/>
@@ -21431,7 +22812,7 @@
       <c r="G40" s="7"/>
       <c r="H40" s="7"/>
     </row>
-    <row r="41" spans="1:8" ht="12.75">
+    <row r="41" spans="1:8" ht="13.2">
       <c r="A41" s="2"/>
       <c r="B41" s="2"/>
       <c r="C41" s="44"/>
@@ -21441,7 +22822,7 @@
       <c r="G41" s="7"/>
       <c r="H41" s="7"/>
     </row>
-    <row r="42" spans="1:8" ht="12.75">
+    <row r="42" spans="1:8" ht="13.2">
       <c r="A42" s="2"/>
       <c r="B42" s="2"/>
       <c r="C42" s="44"/>
@@ -21451,7 +22832,7 @@
       <c r="G42" s="7"/>
       <c r="H42" s="7"/>
     </row>
-    <row r="43" spans="1:8" ht="12.75">
+    <row r="43" spans="1:8" ht="13.2">
       <c r="A43" s="2"/>
       <c r="B43" s="2"/>
       <c r="C43" s="44"/>
@@ -21461,7 +22842,7 @@
       <c r="G43" s="7"/>
       <c r="H43" s="7"/>
     </row>
-    <row r="44" spans="1:8" ht="12.75">
+    <row r="44" spans="1:8" ht="13.2">
       <c r="A44" s="2"/>
       <c r="B44" s="2"/>
       <c r="C44" s="44"/>
@@ -21471,7 +22852,7 @@
       <c r="G44" s="7"/>
       <c r="H44" s="7"/>
     </row>
-    <row r="45" spans="1:8" ht="12.75">
+    <row r="45" spans="1:8" ht="13.2">
       <c r="A45" s="2"/>
       <c r="B45" s="2"/>
       <c r="C45" s="44"/>
@@ -21481,7 +22862,7 @@
       <c r="G45" s="7"/>
       <c r="H45" s="7"/>
     </row>
-    <row r="46" spans="1:8" ht="12.75">
+    <row r="46" spans="1:8" ht="13.2">
       <c r="A46" s="2"/>
       <c r="B46" s="2"/>
       <c r="C46" s="44"/>
@@ -21491,7 +22872,7 @@
       <c r="G46" s="7"/>
       <c r="H46" s="7"/>
     </row>
-    <row r="47" spans="1:8" ht="12.75">
+    <row r="47" spans="1:8" ht="13.2">
       <c r="A47" s="2"/>
       <c r="B47" s="2"/>
       <c r="C47" s="44"/>
@@ -21501,7 +22882,7 @@
       <c r="G47" s="7"/>
       <c r="H47" s="7"/>
     </row>
-    <row r="48" spans="1:8" ht="12.75">
+    <row r="48" spans="1:8" ht="13.2">
       <c r="A48" s="2"/>
       <c r="B48" s="14"/>
       <c r="C48" s="14"/>
@@ -21511,7 +22892,7 @@
       <c r="G48" s="7"/>
       <c r="H48" s="7"/>
     </row>
-    <row r="49" spans="1:8" ht="12.75">
+    <row r="49" spans="1:8" ht="13.2">
       <c r="A49" s="2"/>
       <c r="B49" s="14"/>
       <c r="C49" s="14"/>
@@ -21521,7 +22902,7 @@
       <c r="G49" s="7"/>
       <c r="H49" s="7"/>
     </row>
-    <row r="50" spans="1:8" ht="12.75">
+    <row r="50" spans="1:8" ht="13.2">
       <c r="A50" s="2"/>
       <c r="B50" s="14"/>
       <c r="C50" s="14"/>
@@ -21551,12 +22932,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H34"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="3" max="3" width="14.42578125" style="43"/>
-    <col min="4" max="4" width="17.5703125" customWidth="1"/>
+    <col min="3" max="3" width="14.44140625" style="43"/>
+    <col min="4" max="4" width="17.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" customHeight="1">
@@ -22616,26 +23997,26 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O40"/>
+  <dimension ref="A1:O48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q26" sqref="Q26"/>
+    <sheetView tabSelected="1" topLeftCell="E36" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" customWidth="1"/>
-    <col min="10" max="10" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" customWidth="1"/>
+    <col min="10" max="10" width="15.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="43" customFormat="1">
-      <c r="A1" s="55" t="s">
+      <c r="A1" s="58" t="s">
         <v>208</v>
       </c>
-      <c r="B1" s="56"/>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
+      <c r="B1" s="59"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
     </row>
     <row r="2" spans="1:15">
       <c r="B2" s="31" t="s">
@@ -22676,7 +24057,7 @@
       <c r="M3" s="31" t="s">
         <v>196</v>
       </c>
-      <c r="N3" s="59">
+      <c r="N3" s="53">
         <f>SUM(C24:C26)</f>
         <v>1.0833333333333334E-2</v>
       </c>
@@ -22879,18 +24260,18 @@
       </c>
     </row>
     <row r="22" spans="1:10" ht="35.25" customHeight="1">
-      <c r="A22" s="58" t="s">
+      <c r="A22" s="60" t="s">
         <v>212</v>
       </c>
-      <c r="B22" s="55"/>
-      <c r="C22" s="55"/>
-      <c r="D22" s="55"/>
-      <c r="F22" s="58" t="s">
+      <c r="B22" s="58"/>
+      <c r="C22" s="58"/>
+      <c r="D22" s="58"/>
+      <c r="F22" s="60" t="s">
         <v>214</v>
       </c>
-      <c r="G22" s="55"/>
-      <c r="H22" s="55"/>
-      <c r="I22" s="55"/>
+      <c r="G22" s="58"/>
+      <c r="H22" s="58"/>
+      <c r="I22" s="58"/>
     </row>
     <row r="23" spans="1:10">
       <c r="A23" s="31" t="s">
@@ -22986,7 +24367,7 @@
       <c r="C26" s="48">
         <v>5.0925925925925921E-4</v>
       </c>
-      <c r="D26" s="57">
+      <c r="D26" s="52">
         <v>5.4398148148148144E-4</v>
       </c>
       <c r="E26" s="47"/>
@@ -23161,7 +24542,7 @@
       <c r="C32" s="48">
         <v>4.0509259259259257E-3</v>
       </c>
-      <c r="D32" s="57">
+      <c r="D32" s="52">
         <v>2.6620370370370372E-4</v>
       </c>
       <c r="E32" s="47"/>
@@ -23180,26 +24561,314 @@
         <v>1.3310185185185186E-4</v>
       </c>
     </row>
-    <row r="33" spans="3:5">
+    <row r="33" spans="1:9">
       <c r="C33" s="47"/>
     </row>
-    <row r="34" spans="3:5">
+    <row r="34" spans="1:9">
       <c r="C34" s="47"/>
     </row>
-    <row r="38" spans="3:5">
-      <c r="E38" s="57"/>
-    </row>
-    <row r="39" spans="3:5">
-      <c r="E39" s="57"/>
-    </row>
-    <row r="40" spans="3:5">
-      <c r="E40" s="57"/>
+    <row r="38" spans="1:9">
+      <c r="A38" s="59" t="s">
+        <v>215</v>
+      </c>
+      <c r="B38" s="59"/>
+      <c r="C38" s="59"/>
+      <c r="D38" s="59"/>
+      <c r="E38" s="52"/>
+      <c r="F38" s="59" t="s">
+        <v>216</v>
+      </c>
+      <c r="G38" s="59"/>
+      <c r="H38" s="59"/>
+      <c r="I38" s="59"/>
+    </row>
+    <row r="39" spans="1:9">
+      <c r="A39" t="s">
+        <v>24</v>
+      </c>
+      <c r="B39" t="s">
+        <v>209</v>
+      </c>
+      <c r="C39" t="s">
+        <v>210</v>
+      </c>
+      <c r="D39" t="s">
+        <v>211</v>
+      </c>
+      <c r="E39" s="52"/>
+      <c r="F39" s="51" t="s">
+        <v>24</v>
+      </c>
+      <c r="G39" s="51" t="s">
+        <v>209</v>
+      </c>
+      <c r="H39" s="51" t="s">
+        <v>210</v>
+      </c>
+      <c r="I39" s="51" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9">
+      <c r="A40" s="31" t="s">
+        <v>196</v>
+      </c>
+      <c r="B40" s="31" t="s">
+        <v>185</v>
+      </c>
+      <c r="C40">
+        <v>8</v>
+      </c>
+      <c r="D40">
+        <v>6</v>
+      </c>
+      <c r="E40" s="52"/>
+      <c r="F40" s="31" t="s">
+        <v>196</v>
+      </c>
+      <c r="G40" s="31" t="s">
+        <v>185</v>
+      </c>
+      <c r="H40" s="51">
+        <f>C40/VLOOKUP(G40,$A$17:$B$19,2,)</f>
+        <v>1.3333333333333333</v>
+      </c>
+      <c r="I40" s="51">
+        <f>D40/VLOOKUP(G40,$A$17:$B$19,2,)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9">
+      <c r="A41" s="31" t="s">
+        <v>196</v>
+      </c>
+      <c r="B41" s="31" t="s">
+        <v>186</v>
+      </c>
+      <c r="C41">
+        <v>4</v>
+      </c>
+      <c r="D41">
+        <v>4</v>
+      </c>
+      <c r="F41" s="31" t="s">
+        <v>196</v>
+      </c>
+      <c r="G41" s="31" t="s">
+        <v>186</v>
+      </c>
+      <c r="H41" s="51">
+        <f t="shared" ref="H41:H48" si="2">C41/VLOOKUP(G41,$A$17:$B$19,2,)</f>
+        <v>1.3333333333333333</v>
+      </c>
+      <c r="I41" s="51">
+        <f t="shared" ref="I41:I48" si="3">D41/VLOOKUP(G41,$A$17:$B$19,2,)</f>
+        <v>1.3333333333333333</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9">
+      <c r="A42" s="31" t="s">
+        <v>196</v>
+      </c>
+      <c r="B42" s="31" t="s">
+        <v>187</v>
+      </c>
+      <c r="C42">
+        <v>3</v>
+      </c>
+      <c r="D42">
+        <v>2</v>
+      </c>
+      <c r="F42" s="31" t="s">
+        <v>196</v>
+      </c>
+      <c r="G42" s="31" t="s">
+        <v>187</v>
+      </c>
+      <c r="H42" s="51">
+        <f t="shared" si="2"/>
+        <v>1.5</v>
+      </c>
+      <c r="I42" s="51">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9">
+      <c r="A43" s="31" t="s">
+        <v>197</v>
+      </c>
+      <c r="B43" s="31" t="s">
+        <v>185</v>
+      </c>
+      <c r="C43">
+        <v>12</v>
+      </c>
+      <c r="D43">
+        <v>12</v>
+      </c>
+      <c r="F43" s="31" t="s">
+        <v>197</v>
+      </c>
+      <c r="G43" s="31" t="s">
+        <v>185</v>
+      </c>
+      <c r="H43" s="51">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="I43" s="51">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9">
+      <c r="A44" s="31" t="s">
+        <v>197</v>
+      </c>
+      <c r="B44" s="31" t="s">
+        <v>186</v>
+      </c>
+      <c r="C44">
+        <v>4</v>
+      </c>
+      <c r="D44">
+        <v>5</v>
+      </c>
+      <c r="F44" s="31" t="s">
+        <v>197</v>
+      </c>
+      <c r="G44" s="31" t="s">
+        <v>186</v>
+      </c>
+      <c r="H44" s="51">
+        <f t="shared" si="2"/>
+        <v>1.3333333333333333</v>
+      </c>
+      <c r="I44" s="51">
+        <f t="shared" si="3"/>
+        <v>1.6666666666666667</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9">
+      <c r="A45" s="31" t="s">
+        <v>197</v>
+      </c>
+      <c r="B45" s="31" t="s">
+        <v>187</v>
+      </c>
+      <c r="C45">
+        <v>3</v>
+      </c>
+      <c r="D45">
+        <v>2</v>
+      </c>
+      <c r="F45" s="31" t="s">
+        <v>197</v>
+      </c>
+      <c r="G45" s="31" t="s">
+        <v>187</v>
+      </c>
+      <c r="H45" s="51">
+        <f t="shared" si="2"/>
+        <v>1.5</v>
+      </c>
+      <c r="I45" s="51">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9">
+      <c r="A46" s="31" t="s">
+        <v>198</v>
+      </c>
+      <c r="B46" s="31" t="s">
+        <v>185</v>
+      </c>
+      <c r="C46">
+        <v>10</v>
+      </c>
+      <c r="D46">
+        <v>6</v>
+      </c>
+      <c r="F46" s="31" t="s">
+        <v>198</v>
+      </c>
+      <c r="G46" s="31" t="s">
+        <v>185</v>
+      </c>
+      <c r="H46" s="51">
+        <f t="shared" si="2"/>
+        <v>1.6666666666666667</v>
+      </c>
+      <c r="I46" s="51">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9">
+      <c r="A47" s="31" t="s">
+        <v>198</v>
+      </c>
+      <c r="B47" s="31" t="s">
+        <v>186</v>
+      </c>
+      <c r="C47">
+        <v>6</v>
+      </c>
+      <c r="D47">
+        <v>4</v>
+      </c>
+      <c r="F47" s="31" t="s">
+        <v>198</v>
+      </c>
+      <c r="G47" s="31" t="s">
+        <v>186</v>
+      </c>
+      <c r="H47" s="51">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="I47" s="51">
+        <f t="shared" si="3"/>
+        <v>1.3333333333333333</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9">
+      <c r="A48" s="31" t="s">
+        <v>198</v>
+      </c>
+      <c r="B48" s="31" t="s">
+        <v>187</v>
+      </c>
+      <c r="C48">
+        <v>4</v>
+      </c>
+      <c r="D48">
+        <v>2</v>
+      </c>
+      <c r="F48" s="31" t="s">
+        <v>198</v>
+      </c>
+      <c r="G48" s="31" t="s">
+        <v>187</v>
+      </c>
+      <c r="H48" s="51">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="I48" s="51">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="5">
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A22:D22"/>
     <mergeCell ref="F22:I22"/>
+    <mergeCell ref="A38:D38"/>
+    <mergeCell ref="F38:I38"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -23213,7 +24882,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2"/>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="31" t="s">
@@ -23445,9 +25114,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" s="24" customFormat="1">
@@ -23595,10 +25264,10 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2"/>
   <cols>
-    <col min="1" max="3" width="11.5703125" style="38"/>
-    <col min="9" max="9" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="3" width="11.5546875" style="38"/>
+    <col min="9" max="9" width="16.33203125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="21" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>